<commit_message>
Environment based url for socket
</commit_message>
<xml_diff>
--- a/test-data.xlsx
+++ b/test-data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="23040" windowHeight="9516" tabRatio="644"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="23040" windowHeight="9516" tabRatio="644" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Samedi Compet" sheetId="2" r:id="rId1"/>
@@ -61,12 +61,6 @@
   </si>
   <si>
     <t>Nbre vague</t>
-  </si>
-  <si>
-    <t>Samedi 15 Avril</t>
-  </si>
-  <si>
-    <t>Dimanche 16 Avril</t>
   </si>
   <si>
     <t>Age</t>
@@ -184,6 +178,12 @@
   </si>
   <si>
     <t>Team F</t>
+  </si>
+  <si>
+    <t>Samedi 2 Septembre</t>
+  </si>
+  <si>
+    <t>Dimanche 3 Septembre</t>
   </si>
 </sst>
 </file>
@@ -2978,8 +2978,8 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:M891"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.69921875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2999,7 +2999,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="35" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="B1" s="36"/>
       <c r="C1" s="37"/>
@@ -3037,7 +3037,7 @@
         <v>3</v>
       </c>
       <c r="I2" s="28" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J2" s="20" t="s">
         <v>2</v>
@@ -3060,7 +3060,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H3" s="10" t="s">
         <v>0</v>
@@ -3069,7 +3069,7 @@
         <v>31</v>
       </c>
       <c r="J3" s="31" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K3" s="7">
         <v>1</v>
@@ -3089,7 +3089,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="31" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>0</v>
@@ -3098,7 +3098,7 @@
         <v>24</v>
       </c>
       <c r="J4" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K4" s="3">
         <v>1</v>
@@ -3118,7 +3118,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>0</v>
@@ -3127,7 +3127,7 @@
         <v>36</v>
       </c>
       <c r="J5" s="31" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K5" s="3">
         <v>1</v>
@@ -3147,7 +3147,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="31" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H6" s="10" t="s">
         <v>1</v>
@@ -3156,7 +3156,7 @@
         <v>36</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K6" s="3">
         <v>1</v>
@@ -3176,7 +3176,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="31" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H7" s="10" t="s">
         <v>0</v>
@@ -3185,7 +3185,7 @@
         <v>23</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K7" s="3">
         <v>1</v>
@@ -3205,7 +3205,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="31" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H8" s="10" t="s">
         <v>0</v>
@@ -3214,7 +3214,7 @@
         <v>25</v>
       </c>
       <c r="J8" s="31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K8" s="3">
         <v>1</v>
@@ -3234,7 +3234,7 @@
         <v>2</v>
       </c>
       <c r="G9" s="31" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H9" s="10" t="s">
         <v>1</v>
@@ -3243,7 +3243,7 @@
         <v>24</v>
       </c>
       <c r="J9" s="31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K9" s="3">
         <v>1</v>
@@ -3263,7 +3263,7 @@
         <v>3</v>
       </c>
       <c r="G10" s="31" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H10" s="10" t="s">
         <v>1</v>
@@ -3272,7 +3272,7 @@
         <v>27</v>
       </c>
       <c r="J10" s="31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K10" s="3">
         <v>1</v>
@@ -3292,7 +3292,7 @@
         <v>4</v>
       </c>
       <c r="G11" s="31" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H11" s="10" t="s">
         <v>0</v>
@@ -3301,7 +3301,7 @@
         <v>23</v>
       </c>
       <c r="J11" s="31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K11" s="3">
         <v>1</v>
@@ -3323,7 +3323,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="31" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H12" s="10" t="s">
         <v>0</v>
@@ -3332,7 +3332,7 @@
         <v>31</v>
       </c>
       <c r="J12" s="31" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K12" s="3">
         <v>1</v>
@@ -3354,7 +3354,7 @@
         <v>2</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H13" s="10" t="s">
         <v>0</v>
@@ -3363,7 +3363,7 @@
         <v>16</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K13" s="3">
         <v>1</v>
@@ -3385,7 +3385,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H14" s="10" t="s">
         <v>0</v>
@@ -3394,7 +3394,7 @@
         <v>21</v>
       </c>
       <c r="J14" s="31" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K14" s="3">
         <v>1</v>
@@ -8145,8 +8145,8 @@
   <sheetPr codeName="Feuil4"/>
   <dimension ref="A1:M887"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.69921875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8166,7 +8166,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="35" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="B1" s="36"/>
       <c r="C1" s="37"/>
@@ -8204,7 +8204,7 @@
         <v>3</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J2" s="20" t="s">
         <v>2</v>
@@ -8229,7 +8229,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="32" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H3" s="23" t="s">
         <v>0</v>
@@ -8238,7 +8238,7 @@
         <v>21</v>
       </c>
       <c r="J3" s="33" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K3" s="7">
         <v>1</v>
@@ -8258,7 +8258,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="32" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H4" s="23" t="s">
         <v>0</v>
@@ -8267,7 +8267,7 @@
         <v>22</v>
       </c>
       <c r="J4" s="33" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K4" s="3">
         <v>1</v>
@@ -8287,7 +8287,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="32" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H5" s="23" t="s">
         <v>0</v>
@@ -8296,7 +8296,7 @@
         <v>23</v>
       </c>
       <c r="J5" s="33" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K5" s="3">
         <v>1</v>
@@ -8316,7 +8316,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H6" s="23" t="s">
         <v>0</v>
@@ -8325,7 +8325,7 @@
         <v>24</v>
       </c>
       <c r="J6" s="33" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K6" s="3">
         <v>1</v>
@@ -8345,7 +8345,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="32" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H7" s="23" t="s">
         <v>0</v>
@@ -8354,7 +8354,7 @@
         <v>25</v>
       </c>
       <c r="J7" s="33" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K7" s="3">
         <v>1</v>
@@ -8376,7 +8376,7 @@
         <v>2</v>
       </c>
       <c r="G8" s="32" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H8" s="32" t="s">
         <v>1</v>
@@ -8385,7 +8385,7 @@
         <v>26</v>
       </c>
       <c r="J8" s="33" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K8" s="3">
         <v>1</v>
@@ -8407,7 +8407,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="32" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H9" s="23" t="s">
         <v>0</v>
@@ -8416,7 +8416,7 @@
         <v>27</v>
       </c>
       <c r="J9" s="33" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K9" s="3">
         <v>1</v>
@@ -8438,7 +8438,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="32" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H10" s="23" t="s">
         <v>0</v>
@@ -8447,7 +8447,7 @@
         <v>28</v>
       </c>
       <c r="J10" s="33" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K10" s="3">
         <v>1</v>
@@ -8469,7 +8469,7 @@
         <v>2</v>
       </c>
       <c r="G11" s="32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H11" s="23" t="s">
         <v>0</v>
@@ -8478,7 +8478,7 @@
         <v>29</v>
       </c>
       <c r="J11" s="33" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K11" s="3">
         <v>1</v>
@@ -8500,7 +8500,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="32" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H12" s="23" t="s">
         <v>0</v>
@@ -8509,7 +8509,7 @@
         <v>30</v>
       </c>
       <c r="J12" s="33" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K12" s="3">
         <v>1</v>
@@ -8531,7 +8531,7 @@
         <v>4</v>
       </c>
       <c r="G13" s="32" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H13" s="32" t="s">
         <v>1</v>
@@ -8540,7 +8540,7 @@
         <v>31</v>
       </c>
       <c r="J13" s="33" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K13" s="3">
         <v>1</v>
@@ -8562,7 +8562,7 @@
         <v>5</v>
       </c>
       <c r="G14" s="32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H14" s="23" t="s">
         <v>0</v>
@@ -8571,7 +8571,7 @@
         <v>32</v>
       </c>
       <c r="J14" s="33" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K14" s="3">
         <v>1</v>

</xml_diff>